<commit_message>
Sheet exporter now exports in 3 sections. Removed project total formula from template to prevent it from being duplicated on every row.
</commit_message>
<xml_diff>
--- a/Panoptes/resources/invoiceTemplate.xlsx
+++ b/Panoptes/resources/invoiceTemplate.xlsx
@@ -1320,15 +1320,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>423360</xdr:colOff>
+      <xdr:colOff>450360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>8280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>425520</xdr:colOff>
+      <xdr:colOff>452160</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>145440</xdr:rowOff>
+      <xdr:rowOff>145080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1343,8 +1343,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8688240" y="8280"/>
-          <a:ext cx="1655280" cy="801360"/>
+          <a:off x="8715240" y="8280"/>
+          <a:ext cx="1654920" cy="801000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1367,7 +1367,7 @@
   <dimension ref="A1:AB32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1641,10 +1641,7 @@
         <f aca="false">SUM(E8:K8)</f>
         <v>0</v>
       </c>
-      <c r="M8" s="41" t="n">
-        <f aca="false">SUM(L8:L10)</f>
-        <v>0</v>
-      </c>
+      <c r="M8" s="41"/>
       <c r="N8" s="42"/>
       <c r="O8" s="42"/>
       <c r="P8" s="42"/>
@@ -1749,10 +1746,7 @@
         <f aca="false">SUM(E13:K13)</f>
         <v>0</v>
       </c>
-      <c r="M13" s="41" t="n">
-        <f aca="false">SUM(L13:L16)</f>
-        <v>0</v>
-      </c>
+      <c r="M13" s="41"/>
       <c r="N13" s="42"/>
       <c r="O13" s="42"/>
       <c r="P13" s="42"/>
@@ -1876,10 +1870,7 @@
         <f aca="false">SUM(E19:K19)</f>
         <v>0</v>
       </c>
-      <c r="M19" s="41" t="n">
-        <f aca="false">L19</f>
-        <v>0</v>
-      </c>
+      <c r="M19" s="41"/>
       <c r="N19" s="42"/>
       <c r="O19" s="42"/>
       <c r="P19" s="42"/>

</xml_diff>